<commit_message>
se logra solucionar el problema de bad request
</commit_message>
<xml_diff>
--- a/datosexcel.xlsx
+++ b/datosexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52999\Desktop\Dspace6UploadScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906D2F99-A5D3-48FF-9AE2-3D269EDCE61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9F53D8-5911-4D4B-9E75-F2ACFFB93C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4856,7 +4856,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3152" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3153" uniqueCount="791">
   <si>
     <t>Pertenece a:</t>
   </si>
@@ -9432,6 +9432,9 @@
   </si>
   <si>
     <t>Ex convento de San Antonio de Padua-Izamal</t>
+  </si>
+  <si>
+    <t>San Luis Obispo de Tolosa-Calkiní</t>
   </si>
 </sst>
 </file>
@@ -10020,43 +10023,31 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10071,14 +10062,26 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10505,8 +10508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GZ121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GR2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="GT4" sqref="GT4"/>
+    <sheetView tabSelected="1" topLeftCell="GR96" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="GT102" sqref="GT102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10622,61 +10625,61 @@
     <col min="192" max="199" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="200" max="200" width="125.44140625" style="1" customWidth="1"/>
     <col min="201" max="201" width="81.6640625" style="1" customWidth="1"/>
-    <col min="202" max="202" width="3.5546875" style="1" customWidth="1"/>
+    <col min="202" max="202" width="40.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="203" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:208" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96" t="s">
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="96" t="s">
+      <c r="I1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="96" t="s">
+      <c r="J1" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="112" t="s">
+      <c r="K1" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="101" t="s">
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="102"/>
-      <c r="X1" s="102"/>
-      <c r="Y1" s="96" t="s">
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="104"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="104"/>
+      <c r="X1" s="104"/>
+      <c r="Y1" s="98" t="s">
         <v>194</v>
       </c>
-      <c r="Z1" s="96"/>
-      <c r="AA1" s="96"/>
-      <c r="AB1" s="96"/>
-      <c r="AC1" s="96"/>
-      <c r="AD1" s="96"/>
-      <c r="AE1" s="96"/>
-      <c r="AF1" s="97" t="s">
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98"/>
+      <c r="AC1" s="98"/>
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
+      <c r="AF1" s="99" t="s">
         <v>620</v>
       </c>
       <c r="AG1" s="100"/>
@@ -10684,113 +10687,113 @@
       <c r="AI1" s="100"/>
       <c r="AJ1" s="100"/>
       <c r="AK1" s="100"/>
-      <c r="AL1" s="106" t="s">
+      <c r="AL1" s="110" t="s">
         <v>657</v>
       </c>
-      <c r="AM1" s="99" t="s">
+      <c r="AM1" s="111" t="s">
         <v>179</v>
       </c>
       <c r="AN1" s="100"/>
-      <c r="AO1" s="98"/>
-      <c r="AP1" s="96" t="s">
+      <c r="AO1" s="101"/>
+      <c r="AP1" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="AQ1" s="110" t="s">
+      <c r="AQ1" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="AR1" s="109" t="s">
+      <c r="AR1" s="105" t="s">
         <v>434</v>
       </c>
-      <c r="AS1" s="96"/>
-      <c r="AT1" s="96"/>
-      <c r="AU1" s="96" t="s">
+      <c r="AS1" s="98"/>
+      <c r="AT1" s="98"/>
+      <c r="AU1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="96"/>
-      <c r="AW1" s="96"/>
-      <c r="AX1" s="96"/>
-      <c r="AY1" s="96"/>
-      <c r="AZ1" s="97" t="s">
+      <c r="AV1" s="98"/>
+      <c r="AW1" s="98"/>
+      <c r="AX1" s="98"/>
+      <c r="AY1" s="98"/>
+      <c r="AZ1" s="99" t="s">
         <v>578</v>
       </c>
-      <c r="BA1" s="104"/>
-      <c r="BB1" s="104"/>
-      <c r="BC1" s="104"/>
-      <c r="BD1" s="104"/>
-      <c r="BE1" s="104"/>
-      <c r="BF1" s="104"/>
-      <c r="BG1" s="104"/>
-      <c r="BH1" s="104"/>
-      <c r="BI1" s="104"/>
-      <c r="BJ1" s="104"/>
-      <c r="BK1" s="104"/>
-      <c r="BL1" s="104"/>
-      <c r="BM1" s="104"/>
-      <c r="BN1" s="104"/>
-      <c r="BO1" s="104"/>
-      <c r="BP1" s="104"/>
-      <c r="BQ1" s="104"/>
-      <c r="BR1" s="104"/>
-      <c r="BS1" s="104"/>
-      <c r="BT1" s="104"/>
-      <c r="BU1" s="105"/>
-      <c r="BV1" s="96" t="s">
+      <c r="BA1" s="112"/>
+      <c r="BB1" s="112"/>
+      <c r="BC1" s="112"/>
+      <c r="BD1" s="112"/>
+      <c r="BE1" s="112"/>
+      <c r="BF1" s="112"/>
+      <c r="BG1" s="112"/>
+      <c r="BH1" s="112"/>
+      <c r="BI1" s="112"/>
+      <c r="BJ1" s="112"/>
+      <c r="BK1" s="112"/>
+      <c r="BL1" s="112"/>
+      <c r="BM1" s="112"/>
+      <c r="BN1" s="112"/>
+      <c r="BO1" s="112"/>
+      <c r="BP1" s="112"/>
+      <c r="BQ1" s="112"/>
+      <c r="BR1" s="112"/>
+      <c r="BS1" s="112"/>
+      <c r="BT1" s="112"/>
+      <c r="BU1" s="113"/>
+      <c r="BV1" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="BW1" s="96"/>
-      <c r="BX1" s="96"/>
-      <c r="BY1" s="97" t="s">
+      <c r="BW1" s="98"/>
+      <c r="BX1" s="98"/>
+      <c r="BY1" s="99" t="s">
         <v>702</v>
       </c>
-      <c r="BZ1" s="98"/>
-      <c r="CA1" s="101" t="s">
+      <c r="BZ1" s="101"/>
+      <c r="CA1" s="103" t="s">
         <v>441</v>
       </c>
-      <c r="CB1" s="102"/>
-      <c r="CC1" s="102"/>
-      <c r="CD1" s="102"/>
-      <c r="CE1" s="102"/>
-      <c r="CF1" s="102"/>
-      <c r="CG1" s="102"/>
-      <c r="CH1" s="102"/>
-      <c r="CI1" s="102"/>
-      <c r="CJ1" s="102"/>
-      <c r="CK1" s="102"/>
-      <c r="CL1" s="102"/>
-      <c r="CM1" s="102"/>
-      <c r="CN1" s="102"/>
-      <c r="CO1" s="102"/>
-      <c r="CP1" s="102"/>
-      <c r="CQ1" s="102"/>
-      <c r="CR1" s="102"/>
-      <c r="CS1" s="102"/>
-      <c r="CT1" s="102"/>
-      <c r="CU1" s="102"/>
-      <c r="CV1" s="102"/>
-      <c r="CW1" s="102"/>
-      <c r="CX1" s="102"/>
-      <c r="CY1" s="102"/>
-      <c r="CZ1" s="102"/>
-      <c r="DA1" s="102"/>
-      <c r="DB1" s="102"/>
-      <c r="DC1" s="102"/>
-      <c r="DD1" s="102"/>
-      <c r="DE1" s="102"/>
-      <c r="DF1" s="102"/>
-      <c r="DG1" s="102"/>
-      <c r="DH1" s="102"/>
-      <c r="DI1" s="102"/>
-      <c r="DJ1" s="102"/>
-      <c r="DK1" s="102"/>
-      <c r="DL1" s="103"/>
-      <c r="DM1" s="104" t="s">
+      <c r="CB1" s="104"/>
+      <c r="CC1" s="104"/>
+      <c r="CD1" s="104"/>
+      <c r="CE1" s="104"/>
+      <c r="CF1" s="104"/>
+      <c r="CG1" s="104"/>
+      <c r="CH1" s="104"/>
+      <c r="CI1" s="104"/>
+      <c r="CJ1" s="104"/>
+      <c r="CK1" s="104"/>
+      <c r="CL1" s="104"/>
+      <c r="CM1" s="104"/>
+      <c r="CN1" s="104"/>
+      <c r="CO1" s="104"/>
+      <c r="CP1" s="104"/>
+      <c r="CQ1" s="104"/>
+      <c r="CR1" s="104"/>
+      <c r="CS1" s="104"/>
+      <c r="CT1" s="104"/>
+      <c r="CU1" s="104"/>
+      <c r="CV1" s="104"/>
+      <c r="CW1" s="104"/>
+      <c r="CX1" s="104"/>
+      <c r="CY1" s="104"/>
+      <c r="CZ1" s="104"/>
+      <c r="DA1" s="104"/>
+      <c r="DB1" s="104"/>
+      <c r="DC1" s="104"/>
+      <c r="DD1" s="104"/>
+      <c r="DE1" s="104"/>
+      <c r="DF1" s="104"/>
+      <c r="DG1" s="104"/>
+      <c r="DH1" s="104"/>
+      <c r="DI1" s="104"/>
+      <c r="DJ1" s="104"/>
+      <c r="DK1" s="104"/>
+      <c r="DL1" s="109"/>
+      <c r="DM1" s="112" t="s">
         <v>442</v>
       </c>
-      <c r="DN1" s="104"/>
-      <c r="DO1" s="104"/>
-      <c r="DP1" s="104"/>
-      <c r="DQ1" s="105"/>
-      <c r="DR1" s="99" t="s">
+      <c r="DN1" s="112"/>
+      <c r="DO1" s="112"/>
+      <c r="DP1" s="112"/>
+      <c r="DQ1" s="113"/>
+      <c r="DR1" s="111" t="s">
         <v>439</v>
       </c>
       <c r="DS1" s="100"/>
@@ -10817,8 +10820,8 @@
       <c r="EN1" s="100"/>
       <c r="EO1" s="100"/>
       <c r="EP1" s="100"/>
-      <c r="EQ1" s="98"/>
-      <c r="ER1" s="99" t="s">
+      <c r="EQ1" s="101"/>
+      <c r="ER1" s="111" t="s">
         <v>440</v>
       </c>
       <c r="ES1" s="100"/>
@@ -10837,8 +10840,8 @@
       <c r="FF1" s="100"/>
       <c r="FG1" s="100"/>
       <c r="FH1" s="100"/>
-      <c r="FI1" s="98"/>
-      <c r="FJ1" s="99" t="s">
+      <c r="FI1" s="101"/>
+      <c r="FJ1" s="111" t="s">
         <v>12</v>
       </c>
       <c r="FK1" s="100"/>
@@ -10849,30 +10852,30 @@
       <c r="FP1" s="100"/>
       <c r="FQ1" s="100"/>
       <c r="FR1" s="100"/>
-      <c r="FS1" s="98"/>
-      <c r="FT1" s="96" t="s">
+      <c r="FS1" s="101"/>
+      <c r="FT1" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="FU1" s="96"/>
-      <c r="FV1" s="96"/>
-      <c r="FW1" s="96"/>
-      <c r="FX1" s="96"/>
-      <c r="FY1" s="96" t="s">
+      <c r="FU1" s="98"/>
+      <c r="FV1" s="98"/>
+      <c r="FW1" s="98"/>
+      <c r="FX1" s="98"/>
+      <c r="FY1" s="98" t="s">
         <v>235</v>
       </c>
-      <c r="FZ1" s="96"/>
-      <c r="GA1" s="96"/>
-      <c r="GB1" s="96"/>
-      <c r="GC1" s="96"/>
-      <c r="GD1" s="96"/>
-      <c r="GE1" s="99" t="s">
+      <c r="FZ1" s="98"/>
+      <c r="GA1" s="98"/>
+      <c r="GB1" s="98"/>
+      <c r="GC1" s="98"/>
+      <c r="GD1" s="98"/>
+      <c r="GE1" s="111" t="s">
         <v>293</v>
       </c>
       <c r="GF1" s="100"/>
       <c r="GG1" s="100"/>
       <c r="GH1" s="100"/>
-      <c r="GI1" s="98"/>
-      <c r="GJ1" s="97" t="s">
+      <c r="GI1" s="101"/>
+      <c r="GJ1" s="99" t="s">
         <v>14</v>
       </c>
       <c r="GK1" s="100"/>
@@ -10881,20 +10884,20 @@
       <c r="GN1" s="100"/>
       <c r="GO1" s="100"/>
       <c r="GP1" s="100"/>
-      <c r="GQ1" s="98"/>
-      <c r="GR1" s="108" t="s">
+      <c r="GQ1" s="101"/>
+      <c r="GR1" s="102" t="s">
         <v>438</v>
       </c>
-      <c r="GS1" s="107" t="s">
+      <c r="GS1" s="97" t="s">
         <v>631</v>
       </c>
-      <c r="GT1" s="115" t="s">
+      <c r="GT1" s="96" t="s">
         <v>788</v>
       </c>
     </row>
     <row r="2" spans="1:208" ht="388.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="96"/>
-      <c r="B2" s="96"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="98"/>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
@@ -10910,9 +10913,9 @@
       <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
       <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
@@ -10994,7 +10997,7 @@
       <c r="AK2" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="AL2" s="106"/>
+      <c r="AL2" s="110"/>
       <c r="AM2" s="2" t="s">
         <v>180</v>
       </c>
@@ -11004,8 +11007,8 @@
       <c r="AO2" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="AP2" s="111"/>
-      <c r="AQ2" s="110"/>
+      <c r="AP2" s="107"/>
+      <c r="AQ2" s="106"/>
       <c r="AR2" s="7" t="s">
         <v>15</v>
       </c>
@@ -11474,9 +11477,9 @@
       <c r="GQ2" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="GR2" s="101"/>
-      <c r="GS2" s="107"/>
-      <c r="GT2" s="115"/>
+      <c r="GR2" s="103"/>
+      <c r="GS2" s="97"/>
+      <c r="GT2" s="96"/>
     </row>
     <row r="3" spans="1:208" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
@@ -11733,9 +11736,6 @@
       <c r="GR3" s="80"/>
       <c r="GS3" s="93" t="s">
         <v>689</v>
-      </c>
-      <c r="GT3" s="1" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="4" spans="1:208" ht="97.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -15094,7 +15094,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="17" spans="1:201" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:202" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>69</v>
       </c>
@@ -15366,8 +15366,11 @@
         <v>608</v>
       </c>
       <c r="GS17" s="38"/>
+      <c r="GT17" s="1" t="s">
+        <v>789</v>
+      </c>
     </row>
-    <row r="18" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:202" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>286</v>
       </c>
@@ -15618,7 +15621,7 @@
       </c>
       <c r="GS18" s="38"/>
     </row>
-    <row r="19" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="43" t="s">
         <v>72</v>
       </c>
@@ -15857,7 +15860,7 @@
       </c>
       <c r="GS19" s="46"/>
     </row>
-    <row r="20" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="29" t="s">
         <v>379</v>
       </c>
@@ -16102,7 +16105,7 @@
       <c r="GR20" s="80"/>
       <c r="GS20" s="38"/>
     </row>
-    <row r="21" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
         <v>74</v>
       </c>
@@ -16347,7 +16350,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="22" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="29" t="s">
         <v>76</v>
       </c>
@@ -16598,7 +16601,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="23" spans="1:201" ht="113.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:202" ht="113.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>192</v>
       </c>
@@ -16859,7 +16862,7 @@
       </c>
       <c r="GS23" s="38"/>
     </row>
-    <row r="24" spans="1:201" ht="208.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:202" ht="208.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>193</v>
       </c>
@@ -17126,7 +17129,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="25" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>195</v>
       </c>
@@ -17381,7 +17384,7 @@
       </c>
       <c r="GS25" s="38"/>
     </row>
-    <row r="26" spans="1:201" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:202" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>196</v>
       </c>
@@ -17646,7 +17649,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="27" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>372</v>
       </c>
@@ -17891,7 +17894,7 @@
       <c r="GR27" s="81"/>
       <c r="GS27" s="38"/>
     </row>
-    <row r="28" spans="1:201" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:202" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>366</v>
       </c>
@@ -18150,7 +18153,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="29" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19" t="s">
         <v>371</v>
       </c>
@@ -18397,7 +18400,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="30" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="49" t="s">
         <v>46</v>
       </c>
@@ -18634,7 +18637,7 @@
       <c r="GR30" s="85"/>
       <c r="GS30" s="46"/>
     </row>
-    <row r="31" spans="1:201" ht="194.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:202" ht="194.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>197</v>
       </c>
@@ -18905,7 +18908,7 @@
       </c>
       <c r="GS31" s="38"/>
     </row>
-    <row r="32" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:202" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>406</v>
       </c>
@@ -35232,7 +35235,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="97" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="49" t="s">
         <v>143</v>
       </c>
@@ -35465,7 +35468,7 @@
       <c r="GR97" s="88"/>
       <c r="GS97" s="46"/>
     </row>
-    <row r="98" spans="1:201" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:202" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="15" t="s">
         <v>366</v>
       </c>
@@ -35728,7 +35731,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="99" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="10" t="s">
         <v>145</v>
       </c>
@@ -35973,7 +35976,7 @@
       <c r="GR99" s="81"/>
       <c r="GS99" s="38"/>
     </row>
-    <row r="100" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="19" t="s">
         <v>32</v>
       </c>
@@ -36230,7 +36233,7 @@
       <c r="GR100" s="90"/>
       <c r="GS100" s="38"/>
     </row>
-    <row r="101" spans="1:201" ht="97.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:202" ht="97.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="10" t="s">
         <v>314</v>
       </c>
@@ -36496,8 +36499,11 @@
         <v>615</v>
       </c>
       <c r="GS101" s="38"/>
+      <c r="GT101" s="1" t="s">
+        <v>790</v>
+      </c>
     </row>
-    <row r="102" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:202" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="10" t="s">
         <v>105</v>
       </c>
@@ -36758,7 +36764,7 @@
       </c>
       <c r="GS102" s="38"/>
     </row>
-    <row r="103" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="10" t="s">
         <v>87</v>
       </c>
@@ -37011,7 +37017,7 @@
       </c>
       <c r="GS103" s="38"/>
     </row>
-    <row r="104" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="10" t="s">
         <v>62</v>
       </c>
@@ -37266,7 +37272,7 @@
       <c r="GR104" s="82"/>
       <c r="GS104" s="38"/>
     </row>
-    <row r="105" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:202" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="10" t="s">
         <v>326</v>
       </c>
@@ -37523,7 +37529,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="106" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="10" t="s">
         <v>46</v>
       </c>
@@ -37772,7 +37778,7 @@
       <c r="GR106" s="82"/>
       <c r="GS106" s="38"/>
     </row>
-    <row r="107" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="10" t="s">
         <v>105</v>
       </c>
@@ -38021,7 +38027,7 @@
       </c>
       <c r="GS107" s="38"/>
     </row>
-    <row r="108" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="10" t="s">
         <v>62</v>
       </c>
@@ -38276,7 +38282,7 @@
       </c>
       <c r="GS108" s="38"/>
     </row>
-    <row r="109" spans="1:201" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:202" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="s">
         <v>408</v>
       </c>
@@ -38533,7 +38539,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="110" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="10" t="s">
         <v>62</v>
       </c>
@@ -38778,7 +38784,7 @@
       </c>
       <c r="GS110" s="38"/>
     </row>
-    <row r="111" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:202" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="10" t="s">
         <v>491</v>
       </c>
@@ -39015,7 +39021,7 @@
       </c>
       <c r="GS111" s="38"/>
     </row>
-    <row r="112" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="10" t="s">
         <v>338</v>
       </c>
@@ -40482,6 +40488,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="FY1:GD1"/>
+    <mergeCell ref="BY1:BZ1"/>
+    <mergeCell ref="GE1:GI1"/>
+    <mergeCell ref="ER1:FI1"/>
+    <mergeCell ref="FJ1:FS1"/>
+    <mergeCell ref="DR1:EQ1"/>
+    <mergeCell ref="CA1:DL1"/>
+    <mergeCell ref="DM1:DQ1"/>
+    <mergeCell ref="FT1:FX1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AO1"/>
+    <mergeCell ref="BV1:BX1"/>
+    <mergeCell ref="AZ1:BU1"/>
     <mergeCell ref="GT1:GT2"/>
     <mergeCell ref="GS1:GS2"/>
     <mergeCell ref="A1:A2"/>
@@ -40498,21 +40519,6 @@
     <mergeCell ref="AQ1:AQ2"/>
     <mergeCell ref="AP1:AP2"/>
     <mergeCell ref="Y1:AE1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="AF1:AK1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AO1"/>
-    <mergeCell ref="BV1:BX1"/>
-    <mergeCell ref="AZ1:BU1"/>
-    <mergeCell ref="FY1:GD1"/>
-    <mergeCell ref="BY1:BZ1"/>
-    <mergeCell ref="GE1:GI1"/>
-    <mergeCell ref="ER1:FI1"/>
-    <mergeCell ref="FJ1:FS1"/>
-    <mergeCell ref="DR1:EQ1"/>
-    <mergeCell ref="CA1:DL1"/>
-    <mergeCell ref="DM1:DQ1"/>
-    <mergeCell ref="FT1:FX1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -40699,14 +40705,14 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="114" t="s">
         <v>586</v>
       </c>
-      <c r="B3" s="113"/>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
       <c r="G3" s="78" t="s">
         <v>36</v>
       </c>
@@ -40721,14 +40727,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="115" t="s">
         <v>587</v>
       </c>
-      <c r="B4" s="114"/>
-      <c r="C4" s="114"/>
-      <c r="D4" s="114"/>
-      <c r="E4" s="114"/>
-      <c r="F4" s="114"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
       <c r="G4" s="78" t="s">
         <v>583</v>
       </c>

</xml_diff>

<commit_message>
se agrega las coordenadas
</commit_message>
<xml_diff>
--- a/datosexcel.xlsx
+++ b/datosexcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52999\Desktop\Dspace6UploadScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilberth\Desktop\Dspace6ScriptUADY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9F53D8-5911-4D4B-9E75-F2ACFFB93C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D509A40F-7E62-4870-8704-CA4304A9222A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLA" sheetId="1" r:id="rId1"/>
@@ -4856,7 +4856,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3153" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3155" uniqueCount="793">
   <si>
     <t>Pertenece a:</t>
   </si>
@@ -9435,6 +9435,12 @@
   </si>
   <si>
     <t>San Luis Obispo de Tolosa-Calkiní</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
+    <t>Latitud</t>
   </si>
 </sst>
 </file>
@@ -10023,31 +10029,49 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10058,24 +10082,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -10508,178 +10514,175 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GZ121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GR96" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="GT102" sqref="GT102"/>
+    <sheetView tabSelected="1" topLeftCell="GS85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="GX101" sqref="GX101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" style="1" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="2.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="2.6640625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="2.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="2.6640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="2.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14" max="15" width="2.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="2.85546875" style="1" customWidth="1"/>
     <col min="18" max="18" width="3" style="1" customWidth="1"/>
-    <col min="19" max="19" width="2.5546875" style="1" customWidth="1"/>
-    <col min="20" max="21" width="2.77734375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="2.88671875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="2.77734375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="2.88671875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="2.5703125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="2.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="2.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="2.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="2.85546875" style="1" customWidth="1"/>
     <col min="25" max="25" width="3" style="1" customWidth="1"/>
-    <col min="26" max="26" width="2.88671875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="2.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="2.85546875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="1" customWidth="1"/>
     <col min="28" max="28" width="3" style="1" customWidth="1"/>
-    <col min="29" max="29" width="2.5546875" style="1" customWidth="1"/>
-    <col min="30" max="32" width="2.77734375" style="1" customWidth="1"/>
-    <col min="33" max="34" width="2.6640625" style="1" customWidth="1"/>
-    <col min="35" max="35" width="2.5546875" style="1" customWidth="1"/>
-    <col min="36" max="37" width="2.77734375" style="1" customWidth="1"/>
-    <col min="38" max="38" width="36.77734375" style="1" customWidth="1"/>
-    <col min="39" max="41" width="3.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="29.44140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="2.5703125" style="1" customWidth="1"/>
+    <col min="30" max="34" width="2.7109375" style="1" customWidth="1"/>
+    <col min="35" max="35" width="2.5703125" style="1" customWidth="1"/>
+    <col min="36" max="37" width="2.7109375" style="1" customWidth="1"/>
+    <col min="38" max="38" width="36.7109375" style="1" customWidth="1"/>
+    <col min="39" max="41" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="29.42578125" style="1" customWidth="1"/>
     <col min="43" max="43" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="46" width="3.6640625" style="1" customWidth="1"/>
-    <col min="47" max="47" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="2.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="54" width="3.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="3.21875" style="1" customWidth="1"/>
-    <col min="56" max="56" width="3.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="73" width="3.21875" style="1" customWidth="1"/>
-    <col min="74" max="75" width="3.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="77" max="78" width="4.6640625" style="1" customWidth="1"/>
-    <col min="79" max="79" width="2.6640625" style="1" customWidth="1"/>
-    <col min="80" max="80" width="2.77734375" style="1" customWidth="1"/>
-    <col min="81" max="83" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="85" max="87" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="2.6640625" style="1" customWidth="1"/>
-    <col min="91" max="91" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="92" max="93" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="2.6640625" style="1" customWidth="1"/>
+    <col min="44" max="46" width="3.7109375" style="1" customWidth="1"/>
+    <col min="47" max="47" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="54" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="3.28515625" style="1" customWidth="1"/>
+    <col min="56" max="56" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="73" width="3.28515625" style="1" customWidth="1"/>
+    <col min="74" max="75" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="4.7109375" style="1" customWidth="1"/>
+    <col min="79" max="80" width="2.7109375" style="1" customWidth="1"/>
+    <col min="81" max="83" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="85" max="87" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="2.7109375" style="1" customWidth="1"/>
+    <col min="91" max="91" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="92" max="93" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="2.7109375" style="1" customWidth="1"/>
     <col min="95" max="95" width="5" style="1" customWidth="1"/>
-    <col min="96" max="97" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="98" max="99" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="100" max="103" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="4.77734375" style="1" customWidth="1"/>
-    <col min="106" max="106" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="2.88671875" style="1" customWidth="1"/>
-    <col min="108" max="108" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="110" max="111" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="113" max="115" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="117" max="118" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="4.77734375" style="1" customWidth="1"/>
-    <col min="120" max="122" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="2.6640625" style="1" customWidth="1"/>
-    <col min="124" max="124" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="125" max="126" width="2.6640625" style="1" customWidth="1"/>
-    <col min="127" max="127" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="128" max="129" width="2.6640625" style="1" customWidth="1"/>
-    <col min="130" max="130" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="131" max="133" width="2.6640625" style="1" customWidth="1"/>
-    <col min="134" max="136" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="4.77734375" style="1" customWidth="1"/>
-    <col min="139" max="141" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="2.6640625" style="1" customWidth="1"/>
-    <col min="143" max="143" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="145" max="146" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="2.6640625" style="1" customWidth="1"/>
-    <col min="148" max="148" width="2.77734375" style="1" customWidth="1"/>
-    <col min="149" max="150" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="151" max="154" width="2.6640625" style="1" customWidth="1"/>
-    <col min="155" max="157" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="159" max="161" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="162" max="175" width="2.6640625" style="1" customWidth="1"/>
-    <col min="176" max="177" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="3.5546875" style="1" customWidth="1"/>
-    <col min="179" max="180" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="181" max="182" width="3.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="184" max="185" width="3.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="3.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="2.88671875" style="1" customWidth="1"/>
-    <col min="190" max="190" width="2.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="2.77734375" style="1" customWidth="1"/>
-    <col min="192" max="199" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="125.44140625" style="1" customWidth="1"/>
-    <col min="201" max="201" width="81.6640625" style="1" customWidth="1"/>
-    <col min="202" max="202" width="40.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="96" max="97" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="100" max="103" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="4.7109375" style="1" customWidth="1"/>
+    <col min="106" max="106" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="2.85546875" style="1" customWidth="1"/>
+    <col min="108" max="108" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="110" max="111" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="113" max="115" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="117" max="118" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="4.7109375" style="1" customWidth="1"/>
+    <col min="120" max="122" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="2.7109375" style="1" customWidth="1"/>
+    <col min="124" max="124" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="125" max="126" width="2.7109375" style="1" customWidth="1"/>
+    <col min="127" max="127" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="128" max="129" width="2.7109375" style="1" customWidth="1"/>
+    <col min="130" max="130" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="131" max="133" width="2.7109375" style="1" customWidth="1"/>
+    <col min="134" max="136" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="4.7109375" style="1" customWidth="1"/>
+    <col min="139" max="141" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="2.7109375" style="1" customWidth="1"/>
+    <col min="143" max="143" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="145" max="146" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="147" max="148" width="2.7109375" style="1" customWidth="1"/>
+    <col min="149" max="150" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="151" max="154" width="2.7109375" style="1" customWidth="1"/>
+    <col min="155" max="157" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="159" max="161" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="162" max="175" width="2.7109375" style="1" customWidth="1"/>
+    <col min="176" max="177" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="3.5703125" style="1" customWidth="1"/>
+    <col min="179" max="180" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="181" max="182" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="184" max="185" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="2.85546875" style="1" customWidth="1"/>
+    <col min="190" max="190" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="2.7109375" style="1" customWidth="1"/>
+    <col min="192" max="199" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="125.42578125" style="1" customWidth="1"/>
+    <col min="201" max="201" width="81.7109375" style="1" customWidth="1"/>
+    <col min="202" max="202" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="203" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:208" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="98" t="s">
+    <row r="1" spans="1:208" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98" t="s">
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="98" t="s">
+      <c r="I1" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="98" t="s">
+      <c r="J1" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="108" t="s">
+      <c r="K1" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="109"/>
-      <c r="R1" s="103" t="s">
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
+      <c r="P1" s="102"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="104"/>
-      <c r="T1" s="104"/>
-      <c r="U1" s="104"/>
-      <c r="V1" s="104"/>
-      <c r="W1" s="104"/>
-      <c r="X1" s="104"/>
-      <c r="Y1" s="98" t="s">
+      <c r="S1" s="102"/>
+      <c r="T1" s="102"/>
+      <c r="U1" s="102"/>
+      <c r="V1" s="102"/>
+      <c r="W1" s="102"/>
+      <c r="X1" s="102"/>
+      <c r="Y1" s="96" t="s">
         <v>194</v>
       </c>
-      <c r="Z1" s="98"/>
-      <c r="AA1" s="98"/>
-      <c r="AB1" s="98"/>
-      <c r="AC1" s="98"/>
-      <c r="AD1" s="98"/>
-      <c r="AE1" s="98"/>
-      <c r="AF1" s="99" t="s">
+      <c r="Z1" s="96"/>
+      <c r="AA1" s="96"/>
+      <c r="AB1" s="96"/>
+      <c r="AC1" s="96"/>
+      <c r="AD1" s="96"/>
+      <c r="AE1" s="96"/>
+      <c r="AF1" s="97" t="s">
         <v>620</v>
       </c>
       <c r="AG1" s="100"/>
@@ -10687,113 +10690,113 @@
       <c r="AI1" s="100"/>
       <c r="AJ1" s="100"/>
       <c r="AK1" s="100"/>
-      <c r="AL1" s="110" t="s">
+      <c r="AL1" s="107" t="s">
         <v>657</v>
       </c>
-      <c r="AM1" s="111" t="s">
+      <c r="AM1" s="99" t="s">
         <v>179</v>
       </c>
       <c r="AN1" s="100"/>
-      <c r="AO1" s="101"/>
-      <c r="AP1" s="98" t="s">
+      <c r="AO1" s="98"/>
+      <c r="AP1" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="AQ1" s="106" t="s">
+      <c r="AQ1" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="AR1" s="105" t="s">
+      <c r="AR1" s="111" t="s">
         <v>434</v>
       </c>
-      <c r="AS1" s="98"/>
-      <c r="AT1" s="98"/>
-      <c r="AU1" s="98" t="s">
+      <c r="AS1" s="96"/>
+      <c r="AT1" s="96"/>
+      <c r="AU1" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="98"/>
-      <c r="AW1" s="98"/>
-      <c r="AX1" s="98"/>
-      <c r="AY1" s="98"/>
-      <c r="AZ1" s="99" t="s">
+      <c r="AV1" s="96"/>
+      <c r="AW1" s="96"/>
+      <c r="AX1" s="96"/>
+      <c r="AY1" s="96"/>
+      <c r="AZ1" s="97" t="s">
         <v>578</v>
       </c>
-      <c r="BA1" s="112"/>
-      <c r="BB1" s="112"/>
-      <c r="BC1" s="112"/>
-      <c r="BD1" s="112"/>
-      <c r="BE1" s="112"/>
-      <c r="BF1" s="112"/>
-      <c r="BG1" s="112"/>
-      <c r="BH1" s="112"/>
-      <c r="BI1" s="112"/>
-      <c r="BJ1" s="112"/>
-      <c r="BK1" s="112"/>
-      <c r="BL1" s="112"/>
-      <c r="BM1" s="112"/>
-      <c r="BN1" s="112"/>
-      <c r="BO1" s="112"/>
-      <c r="BP1" s="112"/>
-      <c r="BQ1" s="112"/>
-      <c r="BR1" s="112"/>
-      <c r="BS1" s="112"/>
-      <c r="BT1" s="112"/>
-      <c r="BU1" s="113"/>
-      <c r="BV1" s="98" t="s">
+      <c r="BA1" s="104"/>
+      <c r="BB1" s="104"/>
+      <c r="BC1" s="104"/>
+      <c r="BD1" s="104"/>
+      <c r="BE1" s="104"/>
+      <c r="BF1" s="104"/>
+      <c r="BG1" s="104"/>
+      <c r="BH1" s="104"/>
+      <c r="BI1" s="104"/>
+      <c r="BJ1" s="104"/>
+      <c r="BK1" s="104"/>
+      <c r="BL1" s="104"/>
+      <c r="BM1" s="104"/>
+      <c r="BN1" s="104"/>
+      <c r="BO1" s="104"/>
+      <c r="BP1" s="104"/>
+      <c r="BQ1" s="104"/>
+      <c r="BR1" s="104"/>
+      <c r="BS1" s="104"/>
+      <c r="BT1" s="104"/>
+      <c r="BU1" s="105"/>
+      <c r="BV1" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="BW1" s="98"/>
-      <c r="BX1" s="98"/>
-      <c r="BY1" s="99" t="s">
+      <c r="BW1" s="96"/>
+      <c r="BX1" s="96"/>
+      <c r="BY1" s="97" t="s">
         <v>702</v>
       </c>
-      <c r="BZ1" s="101"/>
-      <c r="CA1" s="103" t="s">
+      <c r="BZ1" s="98"/>
+      <c r="CA1" s="101" t="s">
         <v>441</v>
       </c>
-      <c r="CB1" s="104"/>
-      <c r="CC1" s="104"/>
-      <c r="CD1" s="104"/>
-      <c r="CE1" s="104"/>
-      <c r="CF1" s="104"/>
-      <c r="CG1" s="104"/>
-      <c r="CH1" s="104"/>
-      <c r="CI1" s="104"/>
-      <c r="CJ1" s="104"/>
-      <c r="CK1" s="104"/>
-      <c r="CL1" s="104"/>
-      <c r="CM1" s="104"/>
-      <c r="CN1" s="104"/>
-      <c r="CO1" s="104"/>
-      <c r="CP1" s="104"/>
-      <c r="CQ1" s="104"/>
-      <c r="CR1" s="104"/>
-      <c r="CS1" s="104"/>
-      <c r="CT1" s="104"/>
-      <c r="CU1" s="104"/>
-      <c r="CV1" s="104"/>
-      <c r="CW1" s="104"/>
-      <c r="CX1" s="104"/>
-      <c r="CY1" s="104"/>
-      <c r="CZ1" s="104"/>
-      <c r="DA1" s="104"/>
-      <c r="DB1" s="104"/>
-      <c r="DC1" s="104"/>
-      <c r="DD1" s="104"/>
-      <c r="DE1" s="104"/>
-      <c r="DF1" s="104"/>
-      <c r="DG1" s="104"/>
-      <c r="DH1" s="104"/>
-      <c r="DI1" s="104"/>
-      <c r="DJ1" s="104"/>
-      <c r="DK1" s="104"/>
-      <c r="DL1" s="109"/>
-      <c r="DM1" s="112" t="s">
+      <c r="CB1" s="102"/>
+      <c r="CC1" s="102"/>
+      <c r="CD1" s="102"/>
+      <c r="CE1" s="102"/>
+      <c r="CF1" s="102"/>
+      <c r="CG1" s="102"/>
+      <c r="CH1" s="102"/>
+      <c r="CI1" s="102"/>
+      <c r="CJ1" s="102"/>
+      <c r="CK1" s="102"/>
+      <c r="CL1" s="102"/>
+      <c r="CM1" s="102"/>
+      <c r="CN1" s="102"/>
+      <c r="CO1" s="102"/>
+      <c r="CP1" s="102"/>
+      <c r="CQ1" s="102"/>
+      <c r="CR1" s="102"/>
+      <c r="CS1" s="102"/>
+      <c r="CT1" s="102"/>
+      <c r="CU1" s="102"/>
+      <c r="CV1" s="102"/>
+      <c r="CW1" s="102"/>
+      <c r="CX1" s="102"/>
+      <c r="CY1" s="102"/>
+      <c r="CZ1" s="102"/>
+      <c r="DA1" s="102"/>
+      <c r="DB1" s="102"/>
+      <c r="DC1" s="102"/>
+      <c r="DD1" s="102"/>
+      <c r="DE1" s="102"/>
+      <c r="DF1" s="102"/>
+      <c r="DG1" s="102"/>
+      <c r="DH1" s="102"/>
+      <c r="DI1" s="102"/>
+      <c r="DJ1" s="102"/>
+      <c r="DK1" s="102"/>
+      <c r="DL1" s="103"/>
+      <c r="DM1" s="104" t="s">
         <v>442</v>
       </c>
-      <c r="DN1" s="112"/>
-      <c r="DO1" s="112"/>
-      <c r="DP1" s="112"/>
-      <c r="DQ1" s="113"/>
-      <c r="DR1" s="111" t="s">
+      <c r="DN1" s="104"/>
+      <c r="DO1" s="104"/>
+      <c r="DP1" s="104"/>
+      <c r="DQ1" s="105"/>
+      <c r="DR1" s="99" t="s">
         <v>439</v>
       </c>
       <c r="DS1" s="100"/>
@@ -10820,8 +10823,8 @@
       <c r="EN1" s="100"/>
       <c r="EO1" s="100"/>
       <c r="EP1" s="100"/>
-      <c r="EQ1" s="101"/>
-      <c r="ER1" s="111" t="s">
+      <c r="EQ1" s="98"/>
+      <c r="ER1" s="99" t="s">
         <v>440</v>
       </c>
       <c r="ES1" s="100"/>
@@ -10840,8 +10843,8 @@
       <c r="FF1" s="100"/>
       <c r="FG1" s="100"/>
       <c r="FH1" s="100"/>
-      <c r="FI1" s="101"/>
-      <c r="FJ1" s="111" t="s">
+      <c r="FI1" s="98"/>
+      <c r="FJ1" s="99" t="s">
         <v>12</v>
       </c>
       <c r="FK1" s="100"/>
@@ -10852,30 +10855,30 @@
       <c r="FP1" s="100"/>
       <c r="FQ1" s="100"/>
       <c r="FR1" s="100"/>
-      <c r="FS1" s="101"/>
-      <c r="FT1" s="98" t="s">
+      <c r="FS1" s="98"/>
+      <c r="FT1" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="FU1" s="98"/>
-      <c r="FV1" s="98"/>
-      <c r="FW1" s="98"/>
-      <c r="FX1" s="98"/>
-      <c r="FY1" s="98" t="s">
+      <c r="FU1" s="96"/>
+      <c r="FV1" s="96"/>
+      <c r="FW1" s="96"/>
+      <c r="FX1" s="96"/>
+      <c r="FY1" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="FZ1" s="98"/>
-      <c r="GA1" s="98"/>
-      <c r="GB1" s="98"/>
-      <c r="GC1" s="98"/>
-      <c r="GD1" s="98"/>
-      <c r="GE1" s="111" t="s">
+      <c r="FZ1" s="96"/>
+      <c r="GA1" s="96"/>
+      <c r="GB1" s="96"/>
+      <c r="GC1" s="96"/>
+      <c r="GD1" s="96"/>
+      <c r="GE1" s="99" t="s">
         <v>293</v>
       </c>
       <c r="GF1" s="100"/>
       <c r="GG1" s="100"/>
       <c r="GH1" s="100"/>
-      <c r="GI1" s="101"/>
-      <c r="GJ1" s="99" t="s">
+      <c r="GI1" s="98"/>
+      <c r="GJ1" s="97" t="s">
         <v>14</v>
       </c>
       <c r="GK1" s="100"/>
@@ -10884,20 +10887,20 @@
       <c r="GN1" s="100"/>
       <c r="GO1" s="100"/>
       <c r="GP1" s="100"/>
-      <c r="GQ1" s="101"/>
-      <c r="GR1" s="102" t="s">
+      <c r="GQ1" s="98"/>
+      <c r="GR1" s="110" t="s">
         <v>438</v>
       </c>
-      <c r="GS1" s="97" t="s">
+      <c r="GS1" s="109" t="s">
         <v>631</v>
       </c>
-      <c r="GT1" s="96" t="s">
+      <c r="GT1" s="108" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="2" spans="1:208" ht="388.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
+    <row r="2" spans="1:208" ht="388.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
@@ -10913,9 +10916,9 @@
       <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
       <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
@@ -10997,7 +11000,7 @@
       <c r="AK2" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="AL2" s="110"/>
+      <c r="AL2" s="107"/>
       <c r="AM2" s="2" t="s">
         <v>180</v>
       </c>
@@ -11007,8 +11010,8 @@
       <c r="AO2" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="AP2" s="107"/>
-      <c r="AQ2" s="106"/>
+      <c r="AP2" s="113"/>
+      <c r="AQ2" s="112"/>
       <c r="AR2" s="7" t="s">
         <v>15</v>
       </c>
@@ -11477,11 +11480,17 @@
       <c r="GQ2" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="GR2" s="103"/>
-      <c r="GS2" s="97"/>
-      <c r="GT2" s="96"/>
+      <c r="GR2" s="101"/>
+      <c r="GS2" s="109"/>
+      <c r="GT2" s="108"/>
+      <c r="GU2" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="GV2" s="1" t="s">
+        <v>791</v>
+      </c>
     </row>
-    <row r="3" spans="1:208" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:208" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>32</v>
       </c>
@@ -11738,7 +11747,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="4" spans="1:208" ht="97.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:208" ht="90.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>33</v>
       </c>
@@ -11999,7 +12008,7 @@
       </c>
       <c r="GS4" s="38"/>
     </row>
-    <row r="5" spans="1:208" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:208" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>47</v>
       </c>
@@ -12258,7 +12267,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="6" spans="1:208" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:208" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>154</v>
       </c>
@@ -12519,7 +12528,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="7" spans="1:208" ht="37.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:208" ht="37.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>34</v>
       </c>
@@ -12770,7 +12779,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="8" spans="1:208" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:208" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>45</v>
       </c>
@@ -13023,7 +13032,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="9" spans="1:208" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:208" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>46</v>
       </c>
@@ -13278,7 +13287,7 @@
       </c>
       <c r="GS9" s="38"/>
     </row>
-    <row r="10" spans="1:208" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:208" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>58</v>
       </c>
@@ -13547,7 +13556,7 @@
       </c>
       <c r="GS10" s="38"/>
     </row>
-    <row r="11" spans="1:208" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:208" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>55</v>
       </c>
@@ -13808,7 +13817,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="12" spans="1:208" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:208" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>57</v>
       </c>
@@ -14069,7 +14078,7 @@
       <c r="GR12" s="80"/>
       <c r="GS12" s="38"/>
     </row>
-    <row r="13" spans="1:208" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:208" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>58</v>
       </c>
@@ -14330,7 +14339,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="14" spans="1:208" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:208" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>60</v>
       </c>
@@ -14590,7 +14599,7 @@
       <c r="GY14" s="64"/>
       <c r="GZ14" s="64"/>
     </row>
-    <row r="15" spans="1:208" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:208" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>62</v>
       </c>
@@ -14853,7 +14862,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="16" spans="1:208" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:208" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>154</v>
       </c>
@@ -15094,7 +15103,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="17" spans="1:202" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:204" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>69</v>
       </c>
@@ -15369,8 +15378,14 @@
       <c r="GT17" s="1" t="s">
         <v>789</v>
       </c>
+      <c r="GU17" s="1">
+        <v>20.932645720913801</v>
+      </c>
+      <c r="GV17" s="1">
+        <v>-89.018900974184007</v>
+      </c>
     </row>
-    <row r="18" spans="1:202" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:204" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>286</v>
       </c>
@@ -15621,7 +15636,7 @@
       </c>
       <c r="GS18" s="38"/>
     </row>
-    <row r="19" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="43" t="s">
         <v>72</v>
       </c>
@@ -15860,7 +15875,7 @@
       </c>
       <c r="GS19" s="46"/>
     </row>
-    <row r="20" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>379</v>
       </c>
@@ -16105,7 +16120,7 @@
       <c r="GR20" s="80"/>
       <c r="GS20" s="38"/>
     </row>
-    <row r="21" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>74</v>
       </c>
@@ -16350,7 +16365,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="22" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
         <v>76</v>
       </c>
@@ -16601,7 +16616,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="23" spans="1:202" ht="113.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:204" ht="113.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>192</v>
       </c>
@@ -16862,7 +16877,7 @@
       </c>
       <c r="GS23" s="38"/>
     </row>
-    <row r="24" spans="1:202" ht="208.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:204" ht="192.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>193</v>
       </c>
@@ -17129,7 +17144,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="25" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>195</v>
       </c>
@@ -17384,7 +17399,7 @@
       </c>
       <c r="GS25" s="38"/>
     </row>
-    <row r="26" spans="1:202" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:204" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>196</v>
       </c>
@@ -17649,7 +17664,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="27" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>372</v>
       </c>
@@ -17894,7 +17909,7 @@
       <c r="GR27" s="81"/>
       <c r="GS27" s="38"/>
     </row>
-    <row r="28" spans="1:202" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:204" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>366</v>
       </c>
@@ -18153,7 +18168,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="29" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
         <v>371</v>
       </c>
@@ -18400,7 +18415,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="30" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="49" t="s">
         <v>46</v>
       </c>
@@ -18637,7 +18652,7 @@
       <c r="GR30" s="85"/>
       <c r="GS30" s="46"/>
     </row>
-    <row r="31" spans="1:202" ht="194.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:204" ht="180" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>197</v>
       </c>
@@ -18908,7 +18923,7 @@
       </c>
       <c r="GS31" s="38"/>
     </row>
-    <row r="32" spans="1:202" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:204" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>406</v>
       </c>
@@ -19145,7 +19160,7 @@
       <c r="GR32" s="86"/>
       <c r="GS32" s="38"/>
     </row>
-    <row r="33" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:201" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>383</v>
       </c>
@@ -19398,7 +19413,7 @@
       </c>
       <c r="GS33" s="38"/>
     </row>
-    <row r="34" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:201" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>391</v>
       </c>
@@ -19647,7 +19662,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="35" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:201" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>203</v>
       </c>
@@ -19896,7 +19911,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="36" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:201" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>204</v>
       </c>
@@ -20161,7 +20176,7 @@
       </c>
       <c r="GS36" s="38"/>
     </row>
-    <row r="37" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:201" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>252</v>
       </c>
@@ -20422,7 +20437,7 @@
       </c>
       <c r="GS37" s="38"/>
     </row>
-    <row r="38" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:201" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>222</v>
       </c>
@@ -20677,7 +20692,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="39" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="53" t="s">
         <v>205</v>
       </c>
@@ -20932,7 +20947,7 @@
       </c>
       <c r="GS39" s="38"/>
     </row>
-    <row r="40" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:201" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29" t="s">
         <v>227</v>
       </c>
@@ -21181,7 +21196,7 @@
       <c r="GR40" s="80"/>
       <c r="GS40" s="38"/>
     </row>
-    <row r="41" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:201" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>74</v>
       </c>
@@ -21436,7 +21451,7 @@
       </c>
       <c r="GS41" s="38"/>
     </row>
-    <row r="42" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:201" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>221</v>
       </c>
@@ -21695,7 +21710,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="43" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:201" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>77</v>
       </c>
@@ -21954,7 +21969,7 @@
       </c>
       <c r="GS43" s="38"/>
     </row>
-    <row r="44" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="53" t="s">
         <v>228</v>
       </c>
@@ -22205,7 +22220,7 @@
       <c r="GR44" s="80"/>
       <c r="GS44" s="38"/>
     </row>
-    <row r="45" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:201" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>230</v>
       </c>
@@ -22466,7 +22481,7 @@
       </c>
       <c r="GS45" s="38"/>
     </row>
-    <row r="46" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="53" t="s">
         <v>241</v>
       </c>
@@ -22723,7 +22738,7 @@
       <c r="GR46" s="80"/>
       <c r="GS46" s="38"/>
     </row>
-    <row r="47" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:201" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>268</v>
       </c>
@@ -22972,7 +22987,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="48" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:201" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>266</v>
       </c>
@@ -23223,7 +23238,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="49" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:201" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>283</v>
       </c>
@@ -23476,7 +23491,7 @@
       </c>
       <c r="GS49" s="38"/>
     </row>
-    <row r="50" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="53" t="s">
         <v>192</v>
       </c>
@@ -23729,7 +23744,7 @@
       </c>
       <c r="GS50" s="38"/>
     </row>
-    <row r="51" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:201" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="54" t="s">
         <v>264</v>
       </c>
@@ -23974,7 +23989,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="52" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="53" t="s">
         <v>260</v>
       </c>
@@ -24217,7 +24232,7 @@
       <c r="GR52" s="80"/>
       <c r="GS52" s="38"/>
     </row>
-    <row r="53" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:201" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>262</v>
       </c>
@@ -24466,7 +24481,7 @@
       <c r="GR53" s="80"/>
       <c r="GS53" s="38"/>
     </row>
-    <row r="54" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:201" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>270</v>
       </c>
@@ -24717,7 +24732,7 @@
       </c>
       <c r="GS54" s="38"/>
     </row>
-    <row r="55" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="53" t="s">
         <v>275</v>
       </c>
@@ -24960,7 +24975,7 @@
       <c r="GR55" s="80"/>
       <c r="GS55" s="38"/>
     </row>
-    <row r="56" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="53" t="s">
         <v>278</v>
       </c>
@@ -25201,7 +25216,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="57" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="53" t="s">
         <v>280</v>
       </c>
@@ -25446,7 +25461,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="58" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:201" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
         <v>77</v>
       </c>
@@ -25709,7 +25724,7 @@
       <c r="GR58" s="80"/>
       <c r="GS58" s="38"/>
     </row>
-    <row r="59" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="19" t="s">
         <v>79</v>
       </c>
@@ -25952,7 +25967,7 @@
       <c r="GR59" s="80"/>
       <c r="GS59" s="38"/>
     </row>
-    <row r="60" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:201" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>80</v>
       </c>
@@ -26219,7 +26234,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="61" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="19" t="s">
         <v>82</v>
       </c>
@@ -26468,7 +26483,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="62" spans="1:201" ht="125.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:201" ht="116.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
         <v>58</v>
       </c>
@@ -26737,7 +26752,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="63" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="19" t="s">
         <v>85</v>
       </c>
@@ -26978,7 +26993,7 @@
       <c r="GR63" s="80"/>
       <c r="GS63" s="38"/>
     </row>
-    <row r="64" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="19"/>
       <c r="B64" s="36"/>
       <c r="C64" s="12"/>
@@ -27207,7 +27222,7 @@
       <c r="GR64" s="80"/>
       <c r="GS64" s="38"/>
     </row>
-    <row r="65" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:201" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>298</v>
       </c>
@@ -27456,7 +27471,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="66" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="19" t="s">
         <v>87</v>
       </c>
@@ -27705,7 +27720,7 @@
       <c r="GR66" s="80"/>
       <c r="GS66" s="38"/>
     </row>
-    <row r="67" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="19" t="s">
         <v>88</v>
       </c>
@@ -27956,7 +27971,7 @@
       </c>
       <c r="GS67" s="38"/>
     </row>
-    <row r="68" spans="1:201" ht="103.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:201" ht="103.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
         <v>89</v>
       </c>
@@ -28221,7 +28236,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="69" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="49" t="s">
         <v>91</v>
       </c>
@@ -28462,7 +28477,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="70" spans="1:201" ht="180.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:201" ht="180" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
         <v>299</v>
       </c>
@@ -28719,7 +28734,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="71" spans="1:201" ht="129" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:201" ht="129" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
         <v>105</v>
       </c>
@@ -28980,7 +28995,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="72" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
         <v>46</v>
       </c>
@@ -29229,7 +29244,7 @@
       <c r="GR72" s="90"/>
       <c r="GS72" s="38"/>
     </row>
-    <row r="73" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:201" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
         <v>96</v>
       </c>
@@ -29482,7 +29497,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="74" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="19" t="s">
         <v>427</v>
       </c>
@@ -29737,7 +29752,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="75" spans="1:201" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:201" ht="53.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>98</v>
       </c>
@@ -29998,7 +30013,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="76" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:201" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
         <v>100</v>
       </c>
@@ -30245,7 +30260,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="77" spans="1:201" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:201" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>101</v>
       </c>
@@ -30498,7 +30513,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="78" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="19" t="s">
         <v>103</v>
       </c>
@@ -30749,7 +30764,7 @@
       <c r="GR78" s="90"/>
       <c r="GS78" s="38"/>
     </row>
-    <row r="79" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="19" t="s">
         <v>105</v>
       </c>
@@ -30992,7 +31007,7 @@
       <c r="GR79" s="90"/>
       <c r="GS79" s="38"/>
     </row>
-    <row r="80" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="19" t="s">
         <v>105</v>
       </c>
@@ -31245,7 +31260,7 @@
       </c>
       <c r="GS80" s="38"/>
     </row>
-    <row r="81" spans="1:201" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:201" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="15" t="s">
         <v>121</v>
       </c>
@@ -31512,7 +31527,7 @@
       <c r="GR81" s="90"/>
       <c r="GS81" s="38"/>
     </row>
-    <row r="82" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:201" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="s">
         <v>437</v>
       </c>
@@ -31763,7 +31778,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="83" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="19" t="s">
         <v>435</v>
       </c>
@@ -32002,7 +32017,7 @@
       <c r="GR83" s="90"/>
       <c r="GS83" s="38"/>
     </row>
-    <row r="84" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="19" t="s">
         <v>433</v>
       </c>
@@ -32239,7 +32254,7 @@
       <c r="GR84" s="90"/>
       <c r="GS84" s="38"/>
     </row>
-    <row r="85" spans="1:201" ht="135.30000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:201" ht="135.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
         <v>430</v>
       </c>
@@ -32490,7 +32505,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="86" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="19" t="s">
         <v>377</v>
       </c>
@@ -32743,7 +32758,7 @@
       <c r="GR86" s="90"/>
       <c r="GS86" s="38"/>
     </row>
-    <row r="87" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:201" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="15" t="s">
         <v>125</v>
       </c>
@@ -33000,7 +33015,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="88" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:201" ht="40.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="15" t="s">
         <v>47</v>
       </c>
@@ -33241,7 +33256,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="89" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:201" ht="40.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="10" t="s">
         <v>127</v>
       </c>
@@ -33498,7 +33513,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="90" spans="1:201" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:201" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="15" t="s">
         <v>129</v>
       </c>
@@ -33765,7 +33780,7 @@
       </c>
       <c r="GS90" s="38"/>
     </row>
-    <row r="91" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="49"/>
       <c r="B91" s="49"/>
       <c r="C91" s="46"/>
@@ -33978,7 +33993,7 @@
       <c r="GR91" s="88"/>
       <c r="GS91" s="46"/>
     </row>
-    <row r="92" spans="1:201" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:201" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
         <v>62</v>
       </c>
@@ -34239,7 +34254,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="93" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
         <v>140</v>
       </c>
@@ -34482,7 +34497,7 @@
       <c r="GR93" s="90"/>
       <c r="GS93" s="38"/>
     </row>
-    <row r="94" spans="1:201" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:201" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>222</v>
       </c>
@@ -34717,7 +34732,7 @@
       <c r="GR94" s="90"/>
       <c r="GS94" s="38"/>
     </row>
-    <row r="95" spans="1:201" ht="189" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:201" ht="189" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="10" t="s">
         <v>696</v>
       </c>
@@ -34976,7 +34991,7 @@
       </c>
       <c r="GS95" s="38"/>
     </row>
-    <row r="96" spans="1:201" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:201" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
         <v>378</v>
       </c>
@@ -35235,7 +35250,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="97" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="49" t="s">
         <v>143</v>
       </c>
@@ -35468,7 +35483,7 @@
       <c r="GR97" s="88"/>
       <c r="GS97" s="46"/>
     </row>
-    <row r="98" spans="1:202" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:204" ht="53.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
         <v>366</v>
       </c>
@@ -35731,7 +35746,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="99" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="10" t="s">
         <v>145</v>
       </c>
@@ -35976,7 +35991,7 @@
       <c r="GR99" s="81"/>
       <c r="GS99" s="38"/>
     </row>
-    <row r="100" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="19" t="s">
         <v>32</v>
       </c>
@@ -36233,7 +36248,7 @@
       <c r="GR100" s="90"/>
       <c r="GS100" s="38"/>
     </row>
-    <row r="101" spans="1:202" ht="97.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:204" ht="90.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="10" t="s">
         <v>314</v>
       </c>
@@ -36502,8 +36517,14 @@
       <c r="GT101" s="1" t="s">
         <v>790</v>
       </c>
+      <c r="GU101" s="1">
+        <v>20.3733299503652</v>
+      </c>
+      <c r="GV101" s="1">
+        <v>-90.057746016684206</v>
+      </c>
     </row>
-    <row r="102" spans="1:202" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:204" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="10" t="s">
         <v>105</v>
       </c>
@@ -36764,7 +36785,7 @@
       </c>
       <c r="GS102" s="38"/>
     </row>
-    <row r="103" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="10" t="s">
         <v>87</v>
       </c>
@@ -37017,7 +37038,7 @@
       </c>
       <c r="GS103" s="38"/>
     </row>
-    <row r="104" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="10" t="s">
         <v>62</v>
       </c>
@@ -37272,7 +37293,7 @@
       <c r="GR104" s="82"/>
       <c r="GS104" s="38"/>
     </row>
-    <row r="105" spans="1:202" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:204" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="10" t="s">
         <v>326</v>
       </c>
@@ -37529,7 +37550,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="106" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="10" t="s">
         <v>46</v>
       </c>
@@ -37778,7 +37799,7 @@
       <c r="GR106" s="82"/>
       <c r="GS106" s="38"/>
     </row>
-    <row r="107" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="10" t="s">
         <v>105</v>
       </c>
@@ -38027,7 +38048,7 @@
       </c>
       <c r="GS107" s="38"/>
     </row>
-    <row r="108" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="10" t="s">
         <v>62</v>
       </c>
@@ -38282,7 +38303,7 @@
       </c>
       <c r="GS108" s="38"/>
     </row>
-    <row r="109" spans="1:202" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:204" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="10" t="s">
         <v>408</v>
       </c>
@@ -38539,7 +38560,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="110" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="10" t="s">
         <v>62</v>
       </c>
@@ -38784,7 +38805,7 @@
       </c>
       <c r="GS110" s="38"/>
     </row>
-    <row r="111" spans="1:202" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:204" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="10" t="s">
         <v>491</v>
       </c>
@@ -39021,7 +39042,7 @@
       </c>
       <c r="GS111" s="38"/>
     </row>
-    <row r="112" spans="1:202" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:204" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="10" t="s">
         <v>338</v>
       </c>
@@ -39278,7 +39299,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="113" spans="1:197" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:197" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="AE113" s="64"/>
       <c r="AF113" s="64"/>
       <c r="AG113" s="64"/>
@@ -39434,7 +39455,7 @@
       <c r="GN113" s="65"/>
       <c r="GO113" s="64"/>
     </row>
-    <row r="114" spans="1:197" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:197" x14ac:dyDescent="0.25">
       <c r="A114" s="66" t="s">
         <v>305</v>
       </c>
@@ -39587,7 +39608,7 @@
       <c r="GN114" s="65"/>
       <c r="GO114" s="64"/>
     </row>
-    <row r="115" spans="1:197" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:197" x14ac:dyDescent="0.25">
       <c r="AX115" s="64"/>
       <c r="AY115" s="64"/>
       <c r="AZ115" s="64"/>
@@ -39737,7 +39758,7 @@
       <c r="GN115" s="65"/>
       <c r="GO115" s="64"/>
     </row>
-    <row r="116" spans="1:197" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:197" x14ac:dyDescent="0.25">
       <c r="AX116" s="64"/>
       <c r="AY116" s="64"/>
       <c r="AZ116" s="64"/>
@@ -39886,7 +39907,7 @@
       <c r="GM116" s="65"/>
       <c r="GN116" s="65"/>
     </row>
-    <row r="117" spans="1:197" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:197" x14ac:dyDescent="0.25">
       <c r="CA117" s="65"/>
       <c r="CB117" s="65"/>
       <c r="CC117" s="65"/>
@@ -40006,7 +40027,7 @@
       <c r="GM117" s="65"/>
       <c r="GN117" s="65"/>
     </row>
-    <row r="118" spans="1:197" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:197" x14ac:dyDescent="0.25">
       <c r="CA118" s="65"/>
       <c r="CB118" s="65"/>
       <c r="CC118" s="65"/>
@@ -40126,7 +40147,7 @@
       <c r="GM118" s="65"/>
       <c r="GN118" s="65"/>
     </row>
-    <row r="119" spans="1:197" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:197" x14ac:dyDescent="0.25">
       <c r="CA119" s="65"/>
       <c r="CB119" s="65"/>
       <c r="CC119" s="65"/>
@@ -40246,7 +40267,7 @@
       <c r="GM119" s="65"/>
       <c r="GN119" s="65"/>
     </row>
-    <row r="120" spans="1:197" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:197" x14ac:dyDescent="0.25">
       <c r="CA120" s="65"/>
       <c r="CB120" s="65"/>
       <c r="CC120" s="65"/>
@@ -40366,7 +40387,7 @@
       <c r="GM120" s="65"/>
       <c r="GN120" s="65"/>
     </row>
-    <row r="121" spans="1:197" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:197" x14ac:dyDescent="0.25">
       <c r="CA121" s="65"/>
       <c r="CB121" s="65"/>
       <c r="CC121" s="65"/>
@@ -40488,21 +40509,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="FY1:GD1"/>
-    <mergeCell ref="BY1:BZ1"/>
-    <mergeCell ref="GE1:GI1"/>
-    <mergeCell ref="ER1:FI1"/>
-    <mergeCell ref="FJ1:FS1"/>
-    <mergeCell ref="DR1:EQ1"/>
-    <mergeCell ref="CA1:DL1"/>
-    <mergeCell ref="DM1:DQ1"/>
-    <mergeCell ref="FT1:FX1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="AF1:AK1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AO1"/>
-    <mergeCell ref="BV1:BX1"/>
-    <mergeCell ref="AZ1:BU1"/>
     <mergeCell ref="GT1:GT2"/>
     <mergeCell ref="GS1:GS2"/>
     <mergeCell ref="A1:A2"/>
@@ -40519,6 +40525,21 @@
     <mergeCell ref="AQ1:AQ2"/>
     <mergeCell ref="AP1:AP2"/>
     <mergeCell ref="Y1:AE1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AO1"/>
+    <mergeCell ref="BV1:BX1"/>
+    <mergeCell ref="AZ1:BU1"/>
+    <mergeCell ref="FY1:GD1"/>
+    <mergeCell ref="BY1:BZ1"/>
+    <mergeCell ref="GE1:GI1"/>
+    <mergeCell ref="ER1:FI1"/>
+    <mergeCell ref="FJ1:FS1"/>
+    <mergeCell ref="DR1:EQ1"/>
+    <mergeCell ref="CA1:DL1"/>
+    <mergeCell ref="DM1:DQ1"/>
+    <mergeCell ref="FT1:FX1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -40534,17 +40555,17 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -40552,7 +40573,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>736</v>
       </c>
@@ -40572,7 +40593,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -40586,7 +40607,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>703</v>
       </c>
@@ -40600,12 +40621,12 @@
         <v>743</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>706</v>
       </c>
@@ -40613,7 +40634,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>707</v>
       </c>
@@ -40621,7 +40642,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>708</v>
       </c>
@@ -40629,7 +40650,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>739</v>
       </c>
@@ -40637,7 +40658,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>332</v>
       </c>
@@ -40645,7 +40666,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>749</v>
       </c>
@@ -40653,27 +40674,27 @@
         <v>750</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>759</v>
       </c>
@@ -40692,19 +40713,19 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="114" t="s">
         <v>586</v>
       </c>
@@ -40726,7 +40747,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="115" t="s">
         <v>587</v>
       </c>
@@ -40751,12 +40772,12 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>589</v>
       </c>
@@ -40767,32 +40788,32 @@
         <v>588</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N14" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>722</v>
       </c>
@@ -40800,7 +40821,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>724</v>
       </c>
@@ -40808,7 +40829,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -40816,12 +40837,12 @@
         <v>725</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -40829,7 +40850,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>501</v>
       </c>
@@ -40837,17 +40858,17 @@
         <v>727</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>114</v>
       </c>
@@ -40855,27 +40876,27 @@
         <v>728</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>130</v>
       </c>
@@ -40883,7 +40904,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>429</v>
       </c>
@@ -40891,7 +40912,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>332</v>
       </c>
@@ -40899,67 +40920,67 @@
         <v>594</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N32" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N33" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N34" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N35" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N36" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N37" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="38" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N38" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N39" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="40" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N40" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="41" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N41" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="42" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N42" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="43" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N43" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="44" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N44" t="s">
         <v>605</v>
       </c>
@@ -40983,9 +41004,9 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -40993,12 +41014,12 @@
         <v>518</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>187</v>
       </c>
@@ -41009,7 +41030,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>511</v>
       </c>
@@ -41017,7 +41038,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>445</v>
       </c>
@@ -41025,7 +41046,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>513</v>
       </c>
@@ -41033,7 +41054,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>514</v>
       </c>
@@ -41041,7 +41062,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -41049,7 +41070,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -41057,7 +41078,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -41065,7 +41086,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>221</v>
       </c>
@@ -41073,7 +41094,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>187</v>
       </c>
@@ -41081,7 +41102,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>607</v>
       </c>
@@ -41100,14 +41121,14 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>499</v>
       </c>
@@ -41115,7 +41136,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>500</v>
       </c>
@@ -41123,7 +41144,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>501</v>
       </c>
@@ -41131,7 +41152,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>502</v>
       </c>
@@ -41139,7 +41160,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -41147,7 +41168,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -41155,7 +41176,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>503</v>
       </c>
@@ -41163,7 +41184,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>504</v>
       </c>
@@ -41171,7 +41192,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>322</v>
       </c>
@@ -41179,24 +41200,24 @@
         <v>418</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
         <v>568</v>
       </c>
       <c r="B16" s="72"/>
       <c r="C16" s="72"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
         <v>569</v>
       </c>
@@ -41217,9 +41238,9 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -41227,7 +41248,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>383</v>
       </c>
@@ -41235,7 +41256,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>507</v>
       </c>
@@ -41246,12 +41267,12 @@
         <v>532</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>508</v>
       </c>
@@ -41259,12 +41280,12 @@
         <v>533</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>208</v>
       </c>
@@ -41272,7 +41293,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>510</v>
       </c>
@@ -41280,7 +41301,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -41288,7 +41309,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>313</v>
       </c>
@@ -41296,7 +41317,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>187</v>
       </c>
@@ -41304,7 +41325,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>540</v>
       </c>
@@ -41312,7 +41333,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>542</v>
       </c>
@@ -41330,9 +41351,9 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>469</v>
       </c>
@@ -41340,42 +41361,42 @@
         <v>489</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>477</v>
       </c>
@@ -41393,13 +41414,13 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
         <v>449</v>
       </c>
@@ -41407,7 +41428,7 @@
       <c r="C1" s="72"/>
       <c r="D1" s="72"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="70" t="s">
         <v>27</v>
       </c>
@@ -41422,7 +41443,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>36</v>
       </c>
@@ -41445,7 +41466,7 @@
       </c>
       <c r="O3" s="64"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>48</v>
       </c>
@@ -41466,7 +41487,7 @@
       <c r="N4" s="64"/>
       <c r="O4" s="64"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>49</v>
       </c>
@@ -41487,7 +41508,7 @@
       <c r="N5" s="64"/>
       <c r="O5" s="64"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>301</v>
       </c>
@@ -41506,7 +41527,7 @@
       <c r="N6" s="64"/>
       <c r="O6" s="64"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>370</v>
       </c>
@@ -41529,7 +41550,7 @@
       <c r="N7" s="64"/>
       <c r="O7" s="64"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
         <v>187</v>
       </c>
@@ -41548,7 +41569,7 @@
       <c r="N8" s="64"/>
       <c r="O8" s="64"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
         <v>443</v>
       </c>
@@ -41558,7 +41579,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="64" t="s">
         <v>444</v>
       </c>
@@ -41568,7 +41589,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
         <v>445</v>
       </c>
@@ -41581,7 +41602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="64" t="s">
         <v>446</v>
       </c>
@@ -41591,7 +41612,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
         <v>260</v>
       </c>
@@ -41601,7 +41622,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="64" t="s">
         <v>262</v>
       </c>
@@ -41611,14 +41632,14 @@
         <v>468</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="64" t="s">
         <v>447</v>
       </c>
       <c r="B15" s="64"/>
       <c r="C15" s="64"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="64" t="s">
         <v>211</v>
       </c>
@@ -41640,7 +41661,7 @@
       <c r="O16" s="64"/>
       <c r="P16" s="64"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="64" t="s">
         <v>428</v>
       </c>
@@ -41664,7 +41685,7 @@
       <c r="O17" s="64"/>
       <c r="P17" s="64"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="64" t="s">
         <v>115</v>
       </c>
@@ -41686,7 +41707,7 @@
       <c r="O18" s="64"/>
       <c r="P18" s="64"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="64" t="s">
         <v>448</v>
       </c>
@@ -41706,7 +41727,7 @@
       <c r="O19" s="64"/>
       <c r="P19" s="64"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B20" s="64"/>
       <c r="C20" s="64"/>
       <c r="D20" s="64"/>
@@ -41723,18 +41744,18 @@
       <c r="O20" s="64"/>
       <c r="P20" s="64"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="64" t="s">
         <v>462</v>
       </c>
       <c r="B21" s="64"/>
       <c r="C21" s="64"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="64"/>
       <c r="C22" s="64"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="64" t="s">
         <v>516</v>
       </c>
@@ -41743,7 +41764,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B24" s="64"/>
       <c r="C24" s="64"/>
     </row>

</xml_diff>

<commit_message>
Se agrega longitud y latitud
</commit_message>
<xml_diff>
--- a/datosexcel.xlsx
+++ b/datosexcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilberth\Desktop\Dspace6ScriptUADY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wilberth\Desktop\Dspace6ScriptUADY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D509A40F-7E62-4870-8704-CA4304A9222A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9ACDE88-7E02-438E-9682-63926B059855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLA" sheetId="1" r:id="rId1"/>
@@ -9776,7 +9776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10029,49 +10029,31 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10083,11 +10065,32 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10514,8 +10517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GZ121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GS85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="GX101" sqref="GX101"/>
+    <sheetView tabSelected="1" topLeftCell="GS2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="GW2" sqref="GW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10633,56 +10636,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:208" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96" t="s">
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="96" t="s">
+      <c r="I1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="96" t="s">
+      <c r="J1" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="106" t="s">
+      <c r="K1" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="101" t="s">
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="102"/>
-      <c r="X1" s="102"/>
-      <c r="Y1" s="96" t="s">
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="104"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="104"/>
+      <c r="X1" s="104"/>
+      <c r="Y1" s="98" t="s">
         <v>194</v>
       </c>
-      <c r="Z1" s="96"/>
-      <c r="AA1" s="96"/>
-      <c r="AB1" s="96"/>
-      <c r="AC1" s="96"/>
-      <c r="AD1" s="96"/>
-      <c r="AE1" s="96"/>
-      <c r="AF1" s="97" t="s">
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98"/>
+      <c r="AC1" s="98"/>
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
+      <c r="AF1" s="99" t="s">
         <v>620</v>
       </c>
       <c r="AG1" s="100"/>
@@ -10690,113 +10693,113 @@
       <c r="AI1" s="100"/>
       <c r="AJ1" s="100"/>
       <c r="AK1" s="100"/>
-      <c r="AL1" s="107" t="s">
+      <c r="AL1" s="110" t="s">
         <v>657</v>
       </c>
-      <c r="AM1" s="99" t="s">
+      <c r="AM1" s="111" t="s">
         <v>179</v>
       </c>
       <c r="AN1" s="100"/>
-      <c r="AO1" s="98"/>
-      <c r="AP1" s="96" t="s">
+      <c r="AO1" s="101"/>
+      <c r="AP1" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="AQ1" s="112" t="s">
+      <c r="AQ1" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="AR1" s="111" t="s">
+      <c r="AR1" s="105" t="s">
         <v>434</v>
       </c>
-      <c r="AS1" s="96"/>
-      <c r="AT1" s="96"/>
-      <c r="AU1" s="96" t="s">
+      <c r="AS1" s="98"/>
+      <c r="AT1" s="98"/>
+      <c r="AU1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="96"/>
-      <c r="AW1" s="96"/>
-      <c r="AX1" s="96"/>
-      <c r="AY1" s="96"/>
-      <c r="AZ1" s="97" t="s">
+      <c r="AV1" s="98"/>
+      <c r="AW1" s="98"/>
+      <c r="AX1" s="98"/>
+      <c r="AY1" s="98"/>
+      <c r="AZ1" s="99" t="s">
         <v>578</v>
       </c>
-      <c r="BA1" s="104"/>
-      <c r="BB1" s="104"/>
-      <c r="BC1" s="104"/>
-      <c r="BD1" s="104"/>
-      <c r="BE1" s="104"/>
-      <c r="BF1" s="104"/>
-      <c r="BG1" s="104"/>
-      <c r="BH1" s="104"/>
-      <c r="BI1" s="104"/>
-      <c r="BJ1" s="104"/>
-      <c r="BK1" s="104"/>
-      <c r="BL1" s="104"/>
-      <c r="BM1" s="104"/>
-      <c r="BN1" s="104"/>
-      <c r="BO1" s="104"/>
-      <c r="BP1" s="104"/>
-      <c r="BQ1" s="104"/>
-      <c r="BR1" s="104"/>
-      <c r="BS1" s="104"/>
-      <c r="BT1" s="104"/>
-      <c r="BU1" s="105"/>
-      <c r="BV1" s="96" t="s">
+      <c r="BA1" s="112"/>
+      <c r="BB1" s="112"/>
+      <c r="BC1" s="112"/>
+      <c r="BD1" s="112"/>
+      <c r="BE1" s="112"/>
+      <c r="BF1" s="112"/>
+      <c r="BG1" s="112"/>
+      <c r="BH1" s="112"/>
+      <c r="BI1" s="112"/>
+      <c r="BJ1" s="112"/>
+      <c r="BK1" s="112"/>
+      <c r="BL1" s="112"/>
+      <c r="BM1" s="112"/>
+      <c r="BN1" s="112"/>
+      <c r="BO1" s="112"/>
+      <c r="BP1" s="112"/>
+      <c r="BQ1" s="112"/>
+      <c r="BR1" s="112"/>
+      <c r="BS1" s="112"/>
+      <c r="BT1" s="112"/>
+      <c r="BU1" s="113"/>
+      <c r="BV1" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="BW1" s="96"/>
-      <c r="BX1" s="96"/>
-      <c r="BY1" s="97" t="s">
+      <c r="BW1" s="98"/>
+      <c r="BX1" s="98"/>
+      <c r="BY1" s="99" t="s">
         <v>702</v>
       </c>
-      <c r="BZ1" s="98"/>
-      <c r="CA1" s="101" t="s">
+      <c r="BZ1" s="101"/>
+      <c r="CA1" s="103" t="s">
         <v>441</v>
       </c>
-      <c r="CB1" s="102"/>
-      <c r="CC1" s="102"/>
-      <c r="CD1" s="102"/>
-      <c r="CE1" s="102"/>
-      <c r="CF1" s="102"/>
-      <c r="CG1" s="102"/>
-      <c r="CH1" s="102"/>
-      <c r="CI1" s="102"/>
-      <c r="CJ1" s="102"/>
-      <c r="CK1" s="102"/>
-      <c r="CL1" s="102"/>
-      <c r="CM1" s="102"/>
-      <c r="CN1" s="102"/>
-      <c r="CO1" s="102"/>
-      <c r="CP1" s="102"/>
-      <c r="CQ1" s="102"/>
-      <c r="CR1" s="102"/>
-      <c r="CS1" s="102"/>
-      <c r="CT1" s="102"/>
-      <c r="CU1" s="102"/>
-      <c r="CV1" s="102"/>
-      <c r="CW1" s="102"/>
-      <c r="CX1" s="102"/>
-      <c r="CY1" s="102"/>
-      <c r="CZ1" s="102"/>
-      <c r="DA1" s="102"/>
-      <c r="DB1" s="102"/>
-      <c r="DC1" s="102"/>
-      <c r="DD1" s="102"/>
-      <c r="DE1" s="102"/>
-      <c r="DF1" s="102"/>
-      <c r="DG1" s="102"/>
-      <c r="DH1" s="102"/>
-      <c r="DI1" s="102"/>
-      <c r="DJ1" s="102"/>
-      <c r="DK1" s="102"/>
-      <c r="DL1" s="103"/>
-      <c r="DM1" s="104" t="s">
+      <c r="CB1" s="104"/>
+      <c r="CC1" s="104"/>
+      <c r="CD1" s="104"/>
+      <c r="CE1" s="104"/>
+      <c r="CF1" s="104"/>
+      <c r="CG1" s="104"/>
+      <c r="CH1" s="104"/>
+      <c r="CI1" s="104"/>
+      <c r="CJ1" s="104"/>
+      <c r="CK1" s="104"/>
+      <c r="CL1" s="104"/>
+      <c r="CM1" s="104"/>
+      <c r="CN1" s="104"/>
+      <c r="CO1" s="104"/>
+      <c r="CP1" s="104"/>
+      <c r="CQ1" s="104"/>
+      <c r="CR1" s="104"/>
+      <c r="CS1" s="104"/>
+      <c r="CT1" s="104"/>
+      <c r="CU1" s="104"/>
+      <c r="CV1" s="104"/>
+      <c r="CW1" s="104"/>
+      <c r="CX1" s="104"/>
+      <c r="CY1" s="104"/>
+      <c r="CZ1" s="104"/>
+      <c r="DA1" s="104"/>
+      <c r="DB1" s="104"/>
+      <c r="DC1" s="104"/>
+      <c r="DD1" s="104"/>
+      <c r="DE1" s="104"/>
+      <c r="DF1" s="104"/>
+      <c r="DG1" s="104"/>
+      <c r="DH1" s="104"/>
+      <c r="DI1" s="104"/>
+      <c r="DJ1" s="104"/>
+      <c r="DK1" s="104"/>
+      <c r="DL1" s="109"/>
+      <c r="DM1" s="112" t="s">
         <v>442</v>
       </c>
-      <c r="DN1" s="104"/>
-      <c r="DO1" s="104"/>
-      <c r="DP1" s="104"/>
-      <c r="DQ1" s="105"/>
-      <c r="DR1" s="99" t="s">
+      <c r="DN1" s="112"/>
+      <c r="DO1" s="112"/>
+      <c r="DP1" s="112"/>
+      <c r="DQ1" s="113"/>
+      <c r="DR1" s="111" t="s">
         <v>439</v>
       </c>
       <c r="DS1" s="100"/>
@@ -10823,8 +10826,8 @@
       <c r="EN1" s="100"/>
       <c r="EO1" s="100"/>
       <c r="EP1" s="100"/>
-      <c r="EQ1" s="98"/>
-      <c r="ER1" s="99" t="s">
+      <c r="EQ1" s="101"/>
+      <c r="ER1" s="111" t="s">
         <v>440</v>
       </c>
       <c r="ES1" s="100"/>
@@ -10843,8 +10846,8 @@
       <c r="FF1" s="100"/>
       <c r="FG1" s="100"/>
       <c r="FH1" s="100"/>
-      <c r="FI1" s="98"/>
-      <c r="FJ1" s="99" t="s">
+      <c r="FI1" s="101"/>
+      <c r="FJ1" s="111" t="s">
         <v>12</v>
       </c>
       <c r="FK1" s="100"/>
@@ -10855,30 +10858,30 @@
       <c r="FP1" s="100"/>
       <c r="FQ1" s="100"/>
       <c r="FR1" s="100"/>
-      <c r="FS1" s="98"/>
-      <c r="FT1" s="96" t="s">
+      <c r="FS1" s="101"/>
+      <c r="FT1" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="FU1" s="96"/>
-      <c r="FV1" s="96"/>
-      <c r="FW1" s="96"/>
-      <c r="FX1" s="96"/>
-      <c r="FY1" s="96" t="s">
+      <c r="FU1" s="98"/>
+      <c r="FV1" s="98"/>
+      <c r="FW1" s="98"/>
+      <c r="FX1" s="98"/>
+      <c r="FY1" s="98" t="s">
         <v>235</v>
       </c>
-      <c r="FZ1" s="96"/>
-      <c r="GA1" s="96"/>
-      <c r="GB1" s="96"/>
-      <c r="GC1" s="96"/>
-      <c r="GD1" s="96"/>
-      <c r="GE1" s="99" t="s">
+      <c r="FZ1" s="98"/>
+      <c r="GA1" s="98"/>
+      <c r="GB1" s="98"/>
+      <c r="GC1" s="98"/>
+      <c r="GD1" s="98"/>
+      <c r="GE1" s="111" t="s">
         <v>293</v>
       </c>
       <c r="GF1" s="100"/>
       <c r="GG1" s="100"/>
       <c r="GH1" s="100"/>
-      <c r="GI1" s="98"/>
-      <c r="GJ1" s="97" t="s">
+      <c r="GI1" s="101"/>
+      <c r="GJ1" s="99" t="s">
         <v>14</v>
       </c>
       <c r="GK1" s="100"/>
@@ -10887,20 +10890,26 @@
       <c r="GN1" s="100"/>
       <c r="GO1" s="100"/>
       <c r="GP1" s="100"/>
-      <c r="GQ1" s="98"/>
-      <c r="GR1" s="110" t="s">
+      <c r="GQ1" s="101"/>
+      <c r="GR1" s="102" t="s">
         <v>438</v>
       </c>
-      <c r="GS1" s="109" t="s">
+      <c r="GS1" s="97" t="s">
         <v>631</v>
       </c>
-      <c r="GT1" s="108" t="s">
+      <c r="GT1" s="96" t="s">
         <v>788</v>
+      </c>
+      <c r="GU1" s="116" t="s">
+        <v>792</v>
+      </c>
+      <c r="GV1" s="116" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="2" spans="1:208" ht="388.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96"/>
-      <c r="B2" s="96"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="98"/>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
@@ -10916,9 +10925,9 @@
       <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
       <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
@@ -11000,7 +11009,7 @@
       <c r="AK2" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="AL2" s="107"/>
+      <c r="AL2" s="110"/>
       <c r="AM2" s="2" t="s">
         <v>180</v>
       </c>
@@ -11010,8 +11019,8 @@
       <c r="AO2" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="AP2" s="113"/>
-      <c r="AQ2" s="112"/>
+      <c r="AP2" s="107"/>
+      <c r="AQ2" s="106"/>
       <c r="AR2" s="7" t="s">
         <v>15</v>
       </c>
@@ -11480,15 +11489,11 @@
       <c r="GQ2" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="GR2" s="101"/>
-      <c r="GS2" s="109"/>
-      <c r="GT2" s="108"/>
-      <c r="GU2" s="1" t="s">
-        <v>792</v>
-      </c>
-      <c r="GV2" s="1" t="s">
-        <v>791</v>
-      </c>
+      <c r="GR2" s="103"/>
+      <c r="GS2" s="97"/>
+      <c r="GT2" s="96"/>
+      <c r="GU2" s="116"/>
+      <c r="GV2" s="116"/>
     </row>
     <row r="3" spans="1:208" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -40508,7 +40513,24 @@
       <c r="GN121" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="33">
+    <mergeCell ref="GU1:GU2"/>
+    <mergeCell ref="GV1:GV2"/>
+    <mergeCell ref="FY1:GD1"/>
+    <mergeCell ref="BY1:BZ1"/>
+    <mergeCell ref="GE1:GI1"/>
+    <mergeCell ref="ER1:FI1"/>
+    <mergeCell ref="FJ1:FS1"/>
+    <mergeCell ref="DR1:EQ1"/>
+    <mergeCell ref="CA1:DL1"/>
+    <mergeCell ref="DM1:DQ1"/>
+    <mergeCell ref="FT1:FX1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AO1"/>
+    <mergeCell ref="BV1:BX1"/>
+    <mergeCell ref="AZ1:BU1"/>
     <mergeCell ref="GT1:GT2"/>
     <mergeCell ref="GS1:GS2"/>
     <mergeCell ref="A1:A2"/>
@@ -40525,21 +40547,6 @@
     <mergeCell ref="AQ1:AQ2"/>
     <mergeCell ref="AP1:AP2"/>
     <mergeCell ref="Y1:AE1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="AF1:AK1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AO1"/>
-    <mergeCell ref="BV1:BX1"/>
-    <mergeCell ref="AZ1:BU1"/>
-    <mergeCell ref="FY1:GD1"/>
-    <mergeCell ref="BY1:BZ1"/>
-    <mergeCell ref="GE1:GI1"/>
-    <mergeCell ref="ER1:FI1"/>
-    <mergeCell ref="FJ1:FS1"/>
-    <mergeCell ref="DR1:EQ1"/>
-    <mergeCell ref="CA1:DL1"/>
-    <mergeCell ref="DM1:DQ1"/>
-    <mergeCell ref="FT1:FX1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>